<commit_message>
updated elastic net with macro
</commit_message>
<xml_diff>
--- a/Extension code/Forecasting models/Saved preds/roos.xlsx
+++ b/Extension code/Forecasting models/Saved preds/roos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveeur-my.sharepoint.com/personal/594941jc_eur_nl/Documents/Desktop/BondRiskML/Extension code/Forecasting models/Saved preds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_426513BED3F0515C37592811595ED87656CD4578" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14CADA9B-CA90-4135-818A-6DFCA18CE2F6}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_0121F3BAD3F0D80F7F5B2211595ED87656CD0556" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5057CD5D-00C2-4EFA-8F2A-DE3FF6DE8A90}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t>Regression</t>
   </si>
   <si>
-    <t>FWD</t>
+    <t>Macro</t>
   </si>
   <si>
     <t>2 y</t>
@@ -64,7 +64,7 @@
     <t>10 y</t>
   </si>
   <si>
-    <t>Macro</t>
+    <t>Diff Macro</t>
   </si>
 </sst>
 </file>
@@ -96,19 +96,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,14 +452,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="5" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -495,10 +492,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>-2.0256362565757909E-2</v>
+        <v>-8.6718517308349341E-2</v>
       </c>
       <c r="F2">
-        <v>-2.0256362565757909E-2</v>
+        <v>-8.6718517308349341E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -515,10 +512,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>-2.7458534682455401E-2</v>
+        <v>-0.16065015743601371</v>
       </c>
       <c r="F3">
-        <v>-2.7458534682455401E-2</v>
+        <v>-0.16065015743601371</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -535,10 +532,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>-4.2334293420800417E-2</v>
+        <v>-0.16204747881069831</v>
       </c>
       <c r="F4">
-        <v>-4.2334293420800417E-2</v>
+        <v>-0.16204747881069831</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -555,10 +552,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>-6.1520983103698468E-2</v>
+        <v>-4.4305515890824543E-2</v>
       </c>
       <c r="F5">
-        <v>-6.1520983103698468E-2</v>
+        <v>-4.4305515890824543E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -575,10 +572,10 @@
         <v>12</v>
       </c>
       <c r="E6" s="2">
-        <v>-9.4519608981163517E-2</v>
+        <v>1.557368072007914E-2</v>
       </c>
       <c r="F6">
-        <v>-9.4519608981163517E-2</v>
+        <v>1.557368072007914E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -595,10 +592,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="2">
-        <v>-0.16019433341580541</v>
+        <v>3.4832389203050429E-2</v>
       </c>
       <c r="F7">
-        <v>-0.16019433341580541</v>
+        <v>3.4832389203050429E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -615,10 +612,10 @@
         <v>8</v>
       </c>
       <c r="E8">
-        <v>-2.0256362565757909E-2</v>
+        <v>-8.6718517308349341E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>3.9162651885734423E-2</v>
+        <v>-3.4687201216440762E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -635,10 +632,10 @@
         <v>9</v>
       </c>
       <c r="E9">
-        <v>-2.7458534682455401E-2</v>
+        <v>-0.16065015743601371</v>
       </c>
       <c r="F9" s="2">
-        <v>3.0078080803734971E-2</v>
+        <v>-9.1849610512491964E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -655,10 +652,10 @@
         <v>10</v>
       </c>
       <c r="E10">
-        <v>-4.2334293420800417E-2</v>
+        <v>-0.16204747881069831</v>
       </c>
       <c r="F10" s="2">
-        <v>1.5881838897594869E-2</v>
+        <v>-9.2700950739733168E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -675,10 +672,10 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>-6.1520983103698468E-2</v>
+        <v>-4.4305515890824543E-2</v>
       </c>
       <c r="F11" s="2">
-        <v>-3.0172481735013519E-3</v>
+        <v>-4.7189212148697202E-3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -695,10 +692,10 @@
         <v>12</v>
       </c>
       <c r="E12">
-        <v>-9.4519608981163517E-2</v>
+        <v>1.557368072007914E-2</v>
       </c>
       <c r="F12" s="2">
-        <v>-3.0899046757985719E-2</v>
+        <v>4.0129648583176913E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -715,10 +712,10 @@
         <v>13</v>
       </c>
       <c r="E13">
-        <v>-0.16019433341580541</v>
+        <v>3.4832389203050429E-2</v>
       </c>
       <c r="F13" s="2">
-        <v>-8.2396271429023171E-2</v>
+        <v>6.5269173626472332E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -735,10 +732,10 @@
         <v>8</v>
       </c>
       <c r="E14">
-        <v>-2.0256362565757909E-2</v>
+        <v>-8.6718517308349341E-2</v>
       </c>
       <c r="F14" s="3">
-        <v>6.2345050463858083E-2</v>
+        <v>-2.8903429677464838E-3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -755,10 +752,10 @@
         <v>9</v>
       </c>
       <c r="E15">
-        <v>-2.7458534682455401E-2</v>
+        <v>-0.16065015743601371</v>
       </c>
       <c r="F15" s="3">
-        <v>5.3833375079541002E-2</v>
+        <v>-4.2141068631982533E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -775,10 +772,10 @@
         <v>10</v>
       </c>
       <c r="E16">
-        <v>-4.2334293420800417E-2</v>
+        <v>-0.16204747881069831</v>
       </c>
       <c r="F16" s="3">
-        <v>4.2342931907193397E-2</v>
+        <v>-4.2577528247628622E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -795,10 +792,10 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>-6.1520983103698468E-2</v>
+        <v>-4.4305515890824543E-2</v>
       </c>
       <c r="F17" s="3">
-        <v>2.6737493987180731E-2</v>
+        <v>1.5860862992252419E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -815,10 +812,10 @@
         <v>12</v>
       </c>
       <c r="E18">
-        <v>-9.4519608981163517E-2</v>
+        <v>1.557368072007914E-2</v>
       </c>
       <c r="F18" s="3">
-        <v>6.0610754799340638E-3</v>
+        <v>4.5719357750862777E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -835,10 +832,10 @@
         <v>13</v>
       </c>
       <c r="E19">
-        <v>-0.16019433341580541</v>
+        <v>3.4832389203050429E-2</v>
       </c>
       <c r="F19" s="3">
-        <v>-2.9764528530795031E-2</v>
+        <v>6.9609370233771339E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -855,10 +852,10 @@
         <v>8</v>
       </c>
       <c r="E20">
-        <v>-2.0256362565757909E-2</v>
+        <v>-8.6718517308349341E-2</v>
       </c>
       <c r="F20">
-        <v>4.9290833168613379E-2</v>
+        <v>8.6720574377340265E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -875,10 +872,10 @@
         <v>9</v>
       </c>
       <c r="E21">
-        <v>-2.7458534682455401E-2</v>
+        <v>-0.16065015743601371</v>
       </c>
       <c r="F21">
-        <v>4.3807348144962573E-2</v>
+        <v>-1.1524531794485199E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -895,10 +892,10 @@
         <v>10</v>
       </c>
       <c r="E22">
-        <v>-4.2334293420800417E-2</v>
+        <v>-0.16204747881069831</v>
       </c>
       <c r="F22">
-        <v>3.7048985607995077E-2</v>
+        <v>-1.167721133438393E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -915,10 +912,10 @@
         <v>11</v>
       </c>
       <c r="E23">
-        <v>-6.1520983103698468E-2</v>
+        <v>-4.4305515890824543E-2</v>
       </c>
       <c r="F23">
-        <v>2.7743243378347882E-2</v>
+        <v>1.7433836730542329E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -935,10 +932,10 @@
         <v>12</v>
       </c>
       <c r="E24">
-        <v>-9.4519608981163517E-2</v>
+        <v>1.557368072007914E-2</v>
       </c>
       <c r="F24">
-        <v>1.6360757732595928E-2</v>
+        <v>3.2342808223137183E-2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -955,10 +952,10 @@
         <v>13</v>
       </c>
       <c r="E25">
-        <v>-0.16019433341580541</v>
+        <v>3.4832389203050429E-2</v>
       </c>
       <c r="F25">
-        <v>-2.299104721120715E-3</v>
+        <v>4.7852979024947118E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -975,10 +972,10 @@
         <v>8</v>
       </c>
       <c r="E26" s="2">
-        <v>-0.1031159768732697</v>
+        <v>7.0861189491114862E-2</v>
       </c>
       <c r="F26">
-        <v>-0.1031159768732697</v>
+        <v>7.0861189491114862E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -995,10 +992,10 @@
         <v>9</v>
       </c>
       <c r="E27" s="2">
-        <v>-0.1480034077540662</v>
+        <v>2.6776963755084541E-2</v>
       </c>
       <c r="F27">
-        <v>-0.1480034077540662</v>
+        <v>2.6776963755084541E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1015,10 +1012,10 @@
         <v>10</v>
       </c>
       <c r="E28" s="2">
-        <v>-0.12739825944900221</v>
+        <v>1.9913420412356771E-2</v>
       </c>
       <c r="F28">
-        <v>-0.12739825944900221</v>
+        <v>1.9913420412356771E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1035,10 +1032,10 @@
         <v>11</v>
       </c>
       <c r="E29" s="2">
-        <v>-0.12541873533406789</v>
+        <v>1.4351677564782729E-2</v>
       </c>
       <c r="F29">
-        <v>-0.12541873533406789</v>
+        <v>1.4351677564782729E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1055,10 +1052,10 @@
         <v>12</v>
       </c>
       <c r="E30" s="2">
-        <v>-0.17096151151190539</v>
+        <v>2.37731554988807E-3</v>
       </c>
       <c r="F30">
-        <v>-0.17096151151190539</v>
+        <v>2.37731554988807E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1075,10 +1072,10 @@
         <v>13</v>
       </c>
       <c r="E31" s="2">
-        <v>-0.1257254263545258</v>
+        <v>2.2013466863607278E-2</v>
       </c>
       <c r="F31">
-        <v>-0.1257254263545258</v>
+        <v>2.2013466863607278E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1095,10 +1092,10 @@
         <v>8</v>
       </c>
       <c r="E32">
-        <v>-0.1031159768732697</v>
+        <v>7.0861189491114862E-2</v>
       </c>
       <c r="F32" s="3">
-        <v>-8.7706122326396407E-3</v>
+        <v>0.10122375431612619</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1115,10 +1112,10 @@
         <v>9</v>
       </c>
       <c r="E33">
-        <v>-0.1480034077540662</v>
+        <v>2.6776963755084541E-2</v>
       </c>
       <c r="F33" s="3">
-        <v>-5.4157417456010659E-2</v>
+        <v>6.6240525456253696E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1135,10 +1132,10 @@
         <v>10</v>
       </c>
       <c r="E34">
-        <v>-0.12739825944900221</v>
+        <v>1.9913420412356771E-2</v>
       </c>
       <c r="F34" s="3">
-        <v>-4.6650357394289348E-2</v>
+        <v>6.7759409216745725E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1155,10 +1152,10 @@
         <v>11</v>
       </c>
       <c r="E35">
-        <v>-0.12541873533406789</v>
+        <v>1.4351677564782729E-2</v>
       </c>
       <c r="F35" s="3">
-        <v>-4.5390146525686743E-2</v>
+        <v>6.7195765823916176E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1175,10 +1172,10 @@
         <v>12</v>
       </c>
       <c r="E36">
-        <v>-0.17096151151190539</v>
+        <v>2.37731554988807E-3</v>
       </c>
       <c r="F36" s="3">
-        <v>-6.6220451858885809E-2</v>
+        <v>6.0955922451027211E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1195,10 +1192,10 @@
         <v>13</v>
       </c>
       <c r="E37">
-        <v>-0.1257254263545258</v>
+        <v>2.2013466863607278E-2</v>
       </c>
       <c r="F37" s="3">
-        <v>-1.804292058914703E-2</v>
+        <v>7.9747644268628348E-2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1215,10 +1212,10 @@
         <v>8</v>
       </c>
       <c r="E38">
-        <v>-0.1031159768732697</v>
+        <v>7.0861189491114862E-2</v>
       </c>
       <c r="F38" s="4">
-        <v>3.9863838793115391E-2</v>
+        <v>9.9534411009277624E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1235,10 +1232,10 @@
         <v>9</v>
       </c>
       <c r="E39">
-        <v>-0.1480034077540662</v>
+        <v>2.6776963755084541E-2</v>
       </c>
       <c r="F39" s="4">
-        <v>1.7918139356853931E-3</v>
+        <v>7.493221873079603E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1255,10 +1252,10 @@
         <v>10</v>
       </c>
       <c r="E40">
-        <v>-0.12739825944900221</v>
+        <v>1.9913420412356771E-2</v>
       </c>
       <c r="F40" s="4">
-        <v>1.498653198781952E-3</v>
+        <v>8.038916874948232E-2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1275,10 +1272,10 @@
         <v>11</v>
       </c>
       <c r="E41">
-        <v>-0.12541873533406789</v>
+        <v>1.4351677564782729E-2</v>
       </c>
       <c r="F41" s="4">
-        <v>2.1891722994515921E-3</v>
+        <v>8.2418515649496871E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1295,10 +1292,10 @@
         <v>12</v>
       </c>
       <c r="E42">
-        <v>-0.17096151151190539</v>
+        <v>2.37731554988807E-3</v>
       </c>
       <c r="F42" s="4">
-        <v>-2.8131800558950371E-3</v>
+        <v>8.0085905493092691E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1315,10 +1312,10 @@
         <v>13</v>
       </c>
       <c r="E43">
-        <v>-0.1257254263545258</v>
+        <v>2.2013466863607278E-2</v>
       </c>
       <c r="F43" s="4">
-        <v>3.8805485725066813E-2</v>
+        <v>9.5323458926367399E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1335,10 +1332,10 @@
         <v>8</v>
       </c>
       <c r="E44">
-        <v>-0.1031159768732697</v>
+        <v>7.0861189491114862E-2</v>
       </c>
       <c r="F44">
-        <v>4.2787376203995198E-2</v>
+        <v>6.579315957056886E-2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1355,10 +1352,10 @@
         <v>9</v>
       </c>
       <c r="E45">
-        <v>-0.1480034077540662</v>
+        <v>2.6776963755084541E-2</v>
       </c>
       <c r="F45">
-        <v>1.9844286421022431E-2</v>
+        <v>5.2852043578711323E-2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1375,10 +1372,10 @@
         <v>10</v>
       </c>
       <c r="E46">
-        <v>-0.12739825944900221</v>
+        <v>1.9913420412356771E-2</v>
       </c>
       <c r="F46">
-        <v>1.7048772330211629E-2</v>
+        <v>5.7802699010567227E-2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1395,10 +1392,10 @@
         <v>11</v>
       </c>
       <c r="E47">
-        <v>-0.12541873533406789</v>
+        <v>1.4351677564782729E-2</v>
       </c>
       <c r="F47">
-        <v>1.73192211413471E-2</v>
+        <v>6.0019927041524812E-2</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1415,10 +1412,10 @@
         <v>12</v>
       </c>
       <c r="E48">
-        <v>-0.17096151151190539</v>
+        <v>2.37731554988807E-3</v>
       </c>
       <c r="F48">
-        <v>1.9260303897066681E-2</v>
+        <v>5.9767264676083509E-2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1435,10 +1432,10 @@
         <v>13</v>
       </c>
       <c r="E49">
-        <v>-0.1257254263545258</v>
+        <v>2.2013466863607278E-2</v>
       </c>
       <c r="F49">
-        <v>4.4819792588115637E-2</v>
+        <v>6.8740910836824543E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>